<commit_message>
[docs] update static analysis v0.5.0 flawfinder
update static analysis v0.5.0 flawfinder
</commit_message>
<xml_diff>
--- a/docs/09_static_analysis/static_analysis_20210614_v0.5.0_reviewed.xlsx
+++ b/docs/09_static_analysis/static_analysis_20210614_v0.5.0_reviewed.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\cmu_project\docs\09_static_analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\study\security\cmu\temp\cmu_project\docs\09_static_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="655" uniqueCount="214">
   <si>
     <t>File</t>
   </si>
@@ -483,9 +483,6 @@
     <t>../cmu_project/source/custom/two-way-ssl-c/server.c:157:  [2] (buffer) char:</t>
   </si>
   <si>
-    <t>../cmu_project/source/custom/two-way-ssl-c/server.c:171:  [2] (integer) atoi:</t>
-  </si>
-  <si>
     <t>../cmu_project/source/server/src/baseEngine.cpp:92:  [2] (misc) open:</t>
   </si>
   <si>
@@ -596,82 +593,115 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>open</t>
+    <t>s</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>../cmu_project/source/common/TcpSendRecvJpeg.cpp:123:  [2] (buffer) memcpy:</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>../cmu_project/source/server/src/pnet_rt.cpp:41:  [2] (misc) open:</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>../cmu_project/source/common/TcpSendRecvJpeg.cpp:99:  [1] (buffer) strlen:</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>n</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>n</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>전체</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Open</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">closed </t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>오검출</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>not a bug</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>g_snprintf</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>be careful</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>close</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>status</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>add exception</t>
+    <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
     <t>open</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>s</t>
+    <t>check range</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>s</t>
+    <t>../cmu_project/source/custom/two-way-ssl-c/server.c:171:  [2] (integer) atoi:</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>s</t>
+    <t>refer ../cmu_project/source/custom/two-way-ssl-c/server.c:171:  [2] (integer) atoi:</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>s</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>../cmu_project/source/common/TcpSendRecvJpeg.cpp:123:  [2] (buffer) memcpy:</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>../cmu_project/source/server/src/pnet_rt.cpp:41:  [2] (misc) open:</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>../cmu_project/source/common/TcpSendRecvJpeg.cpp:99:  [1] (buffer) strlen:</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>n</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>n</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>read</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>전체</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Open</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">closed </t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>오검출</t>
+    <t>don't calculate twice</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1630,7 +1660,7 @@
   <dimension ref="A1:G101"/>
   <sheetViews>
     <sheetView topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="A110" sqref="A110"/>
+      <selection activeCell="A103" sqref="A103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3376,8 +3406,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:W142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="F137" sqref="F137"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3392,13 +3422,16 @@
   <sheetData>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>178</v>
+      </c>
+      <c r="C4" t="s">
         <v>179</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
+        <v>207</v>
+      </c>
+      <c r="E4" t="s">
         <v>180</v>
-      </c>
-      <c r="E4" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -3406,10 +3439,16 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>183</v>
+        <v>182</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="E5" t="s">
+        <v>203</v>
       </c>
       <c r="F5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -3440,7 +3479,13 @@
         <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>183</v>
+        <v>182</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="E10" t="s">
+        <v>203</v>
       </c>
       <c r="F10" t="s">
         <v>145</v>
@@ -3471,7 +3516,10 @@
         <v>3</v>
       </c>
       <c r="C15" t="s">
-        <v>183</v>
+        <v>182</v>
+      </c>
+      <c r="E15" t="s">
+        <v>204</v>
       </c>
       <c r="F15" t="s">
         <v>146</v>
@@ -3502,7 +3550,10 @@
         <v>4</v>
       </c>
       <c r="C20" t="s">
-        <v>183</v>
+        <v>182</v>
+      </c>
+      <c r="E20" t="s">
+        <v>204</v>
       </c>
       <c r="F20" t="s">
         <v>147</v>
@@ -3533,7 +3584,10 @@
         <v>5</v>
       </c>
       <c r="C25" t="s">
-        <v>183</v>
+        <v>182</v>
+      </c>
+      <c r="E25" t="s">
+        <v>204</v>
       </c>
       <c r="F25" t="s">
         <v>148</v>
@@ -3564,10 +3618,16 @@
         <v>6</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>205</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="31" spans="2:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -3585,7 +3645,13 @@
         <v>7</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>205</v>
       </c>
       <c r="F33" s="3" t="s">
         <v>149</v>
@@ -3607,7 +3673,13 @@
         <v>8</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="E36" t="s">
+        <v>203</v>
       </c>
       <c r="F36" s="3" t="s">
         <v>150</v>
@@ -3639,7 +3711,13 @@
         <v>9</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="E41" t="s">
+        <v>203</v>
       </c>
       <c r="F41" s="3" t="s">
         <v>151</v>
@@ -3670,10 +3748,16 @@
         <v>10</v>
       </c>
       <c r="C46" t="s">
-        <v>183</v>
+        <v>182</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="E46" t="s">
+        <v>203</v>
       </c>
       <c r="F46" t="s">
-        <v>152</v>
+        <v>211</v>
       </c>
     </row>
     <row r="47" spans="2:23" x14ac:dyDescent="0.3">
@@ -3686,103 +3770,121 @@
         <v>109</v>
       </c>
     </row>
-    <row r="49" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:14" x14ac:dyDescent="0.3">
       <c r="F49" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="50" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:14" x14ac:dyDescent="0.3">
       <c r="F50" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="51" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B51">
         <v>11</v>
       </c>
       <c r="C51" t="s">
-        <v>186</v>
+        <v>185</v>
+      </c>
+      <c r="D51" t="s">
+        <v>209</v>
+      </c>
+      <c r="E51" t="s">
+        <v>208</v>
       </c>
       <c r="F51" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="52" spans="2:6" x14ac:dyDescent="0.3">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="52" spans="2:14" x14ac:dyDescent="0.3">
       <c r="F52" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="53" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:14" x14ac:dyDescent="0.3">
       <c r="F53" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="54" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:14" x14ac:dyDescent="0.3">
       <c r="F54" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="55" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:14" x14ac:dyDescent="0.3">
       <c r="F55" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="56" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B56">
         <v>12</v>
       </c>
       <c r="C56" t="s">
-        <v>195</v>
+        <v>192</v>
+      </c>
+      <c r="D56" t="s">
+        <v>209</v>
       </c>
       <c r="E56" t="s">
-        <v>188</v>
+        <v>208</v>
       </c>
       <c r="F56" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="57" spans="2:6" x14ac:dyDescent="0.3">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="57" spans="2:14" x14ac:dyDescent="0.3">
       <c r="F57" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="58" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:14" x14ac:dyDescent="0.3">
       <c r="F58" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="59" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:14" x14ac:dyDescent="0.3">
       <c r="F59" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="60" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:14" x14ac:dyDescent="0.3">
       <c r="F60" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="61" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B61">
         <v>13</v>
       </c>
       <c r="C61" t="s">
-        <v>189</v>
+        <v>186</v>
+      </c>
+      <c r="D61" t="s">
+        <v>209</v>
+      </c>
+      <c r="E61" t="s">
+        <v>210</v>
       </c>
       <c r="F61" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="62" spans="2:6" x14ac:dyDescent="0.3">
+        <v>154</v>
+      </c>
+      <c r="N61" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="62" spans="2:14" x14ac:dyDescent="0.3">
       <c r="F62" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="63" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:14" x14ac:dyDescent="0.3">
       <c r="F63" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="64" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:14" x14ac:dyDescent="0.3">
       <c r="F64" t="s">
         <v>110</v>
       </c>
@@ -3797,10 +3899,16 @@
         <v>14</v>
       </c>
       <c r="C66" t="s">
-        <v>190</v>
+        <v>187</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="E66" s="3" t="s">
+        <v>205</v>
       </c>
       <c r="F66" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="67" spans="2:6" x14ac:dyDescent="0.3">
@@ -3818,10 +3926,16 @@
         <v>15</v>
       </c>
       <c r="C69" t="s">
-        <v>191</v>
+        <v>188</v>
+      </c>
+      <c r="D69" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="E69" s="3" t="s">
+        <v>205</v>
       </c>
       <c r="F69" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="70" spans="2:6" x14ac:dyDescent="0.3">
@@ -3839,13 +3953,16 @@
         <v>16</v>
       </c>
       <c r="C72" t="s">
-        <v>192</v>
+        <v>189</v>
+      </c>
+      <c r="D72" t="s">
+        <v>209</v>
       </c>
       <c r="E72" t="s">
-        <v>188</v>
+        <v>208</v>
       </c>
       <c r="F72" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="73" spans="2:6" x14ac:dyDescent="0.3">
@@ -3873,13 +3990,16 @@
         <v>17</v>
       </c>
       <c r="C77" t="s">
-        <v>186</v>
+        <v>185</v>
+      </c>
+      <c r="D77" t="s">
+        <v>209</v>
       </c>
       <c r="E77" t="s">
-        <v>187</v>
+        <v>208</v>
       </c>
       <c r="F77" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="78" spans="2:6" x14ac:dyDescent="0.3">
@@ -3907,20 +4027,26 @@
         <v>18</v>
       </c>
       <c r="C82" t="s">
-        <v>183</v>
+        <v>182</v>
+      </c>
+      <c r="D82" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="E82" t="s">
+        <v>203</v>
       </c>
       <c r="F82" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="83" spans="2:23" x14ac:dyDescent="0.3">
       <c r="F83" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="84" spans="2:23" x14ac:dyDescent="0.3">
       <c r="F84" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="85" spans="2:23" x14ac:dyDescent="0.3">
@@ -3928,20 +4054,26 @@
         <v>19</v>
       </c>
       <c r="C85" t="s">
-        <v>183</v>
+        <v>182</v>
+      </c>
+      <c r="D85" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="E85" t="s">
+        <v>203</v>
       </c>
       <c r="F85" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="86" spans="2:23" x14ac:dyDescent="0.3">
       <c r="F86" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="87" spans="2:23" x14ac:dyDescent="0.3">
       <c r="F87" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="88" spans="2:23" x14ac:dyDescent="0.3">
@@ -3949,20 +4081,26 @@
         <v>20</v>
       </c>
       <c r="C88" t="s">
-        <v>183</v>
+        <v>182</v>
+      </c>
+      <c r="D88" t="s">
+        <v>209</v>
+      </c>
+      <c r="E88" t="s">
+        <v>213</v>
       </c>
       <c r="F88" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="89" spans="2:23" x14ac:dyDescent="0.3">
       <c r="F89" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="90" spans="2:23" x14ac:dyDescent="0.3">
       <c r="F90" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="91" spans="2:23" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -3970,21 +4108,27 @@
         <v>21</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
+      </c>
+      <c r="D91" t="s">
+        <v>209</v>
+      </c>
+      <c r="E91" t="s">
+        <v>213</v>
       </c>
       <c r="F91" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="W91" s="4"/>
     </row>
     <row r="92" spans="2:23" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F92" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="93" spans="2:23" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F93" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="94" spans="2:23" x14ac:dyDescent="0.3">
@@ -3992,20 +4136,26 @@
         <v>22</v>
       </c>
       <c r="C94" t="s">
-        <v>183</v>
+        <v>182</v>
+      </c>
+      <c r="D94" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="E94" t="s">
+        <v>203</v>
       </c>
       <c r="F94" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="95" spans="2:23" x14ac:dyDescent="0.3">
       <c r="F95" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="96" spans="2:23" x14ac:dyDescent="0.3">
       <c r="F96" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="97" spans="2:6" x14ac:dyDescent="0.3">
@@ -4013,20 +4163,26 @@
         <v>23</v>
       </c>
       <c r="C97" t="s">
-        <v>198</v>
+        <v>195</v>
+      </c>
+      <c r="D97" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="E97" t="s">
+        <v>203</v>
       </c>
       <c r="F97" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="98" spans="2:6" x14ac:dyDescent="0.3">
       <c r="F98" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="99" spans="2:6" x14ac:dyDescent="0.3">
       <c r="F99" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="100" spans="2:6" x14ac:dyDescent="0.3">
@@ -4034,20 +4190,26 @@
         <v>24</v>
       </c>
       <c r="C100" t="s">
-        <v>183</v>
+        <v>182</v>
+      </c>
+      <c r="D100" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="E100" t="s">
+        <v>203</v>
       </c>
       <c r="F100" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="101" spans="2:6" x14ac:dyDescent="0.3">
       <c r="F101" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="102" spans="2:6" x14ac:dyDescent="0.3">
       <c r="F102" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="103" spans="2:6" x14ac:dyDescent="0.3">
@@ -4055,20 +4217,26 @@
         <v>25</v>
       </c>
       <c r="C103" t="s">
-        <v>183</v>
+        <v>182</v>
+      </c>
+      <c r="D103" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="E103" t="s">
+        <v>203</v>
       </c>
       <c r="F103" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="104" spans="2:6" x14ac:dyDescent="0.3">
       <c r="F104" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="105" spans="2:6" x14ac:dyDescent="0.3">
       <c r="F105" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="106" spans="2:6" x14ac:dyDescent="0.3">
@@ -4076,20 +4244,26 @@
         <v>26</v>
       </c>
       <c r="C106" t="s">
-        <v>199</v>
+        <v>196</v>
+      </c>
+      <c r="D106" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="E106" t="s">
+        <v>203</v>
       </c>
       <c r="F106" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="107" spans="2:6" x14ac:dyDescent="0.3">
       <c r="F107" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="108" spans="2:6" x14ac:dyDescent="0.3">
       <c r="F108" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="109" spans="2:6" x14ac:dyDescent="0.3">
@@ -4097,13 +4271,16 @@
         <v>27</v>
       </c>
       <c r="C109" t="s">
-        <v>200</v>
+        <v>197</v>
+      </c>
+      <c r="D109" t="s">
+        <v>209</v>
       </c>
       <c r="E109" t="s">
-        <v>201</v>
+        <v>208</v>
       </c>
       <c r="F109" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="110" spans="2:6" x14ac:dyDescent="0.3">
@@ -4121,13 +4298,16 @@
         <v>28</v>
       </c>
       <c r="C112" t="s">
-        <v>202</v>
+        <v>198</v>
+      </c>
+      <c r="D112" t="s">
+        <v>209</v>
       </c>
       <c r="E112" t="s">
-        <v>201</v>
+        <v>208</v>
       </c>
       <c r="F112" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="113" spans="2:6" x14ac:dyDescent="0.3">
@@ -4145,13 +4325,16 @@
         <v>29</v>
       </c>
       <c r="C115" t="s">
-        <v>191</v>
+        <v>188</v>
+      </c>
+      <c r="D115" t="s">
+        <v>209</v>
       </c>
       <c r="E115" t="s">
-        <v>201</v>
+        <v>208</v>
       </c>
       <c r="F115" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="116" spans="2:6" x14ac:dyDescent="0.3">
@@ -4169,10 +4352,16 @@
         <v>30</v>
       </c>
       <c r="C118" t="s">
-        <v>186</v>
+        <v>185</v>
+      </c>
+      <c r="D118" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="E118" t="s">
+        <v>203</v>
       </c>
       <c r="F118" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="119" spans="2:6" x14ac:dyDescent="0.3">
@@ -4190,10 +4379,16 @@
         <v>31</v>
       </c>
       <c r="C121" t="s">
-        <v>186</v>
+        <v>185</v>
+      </c>
+      <c r="D121" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="E121" t="s">
+        <v>203</v>
       </c>
       <c r="F121" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="122" spans="2:6" x14ac:dyDescent="0.3">
@@ -4211,10 +4406,16 @@
         <v>32</v>
       </c>
       <c r="C124" t="s">
-        <v>190</v>
+        <v>187</v>
+      </c>
+      <c r="D124" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="E124" t="s">
+        <v>203</v>
       </c>
       <c r="F124" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="125" spans="2:6" x14ac:dyDescent="0.3">
@@ -4232,10 +4433,16 @@
         <v>33</v>
       </c>
       <c r="C127" t="s">
-        <v>193</v>
+        <v>190</v>
+      </c>
+      <c r="D127" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="E127" t="s">
+        <v>203</v>
       </c>
       <c r="F127" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="128" spans="2:6" x14ac:dyDescent="0.3">
@@ -4253,10 +4460,16 @@
         <v>34</v>
       </c>
       <c r="C130" t="s">
-        <v>190</v>
+        <v>187</v>
+      </c>
+      <c r="D130" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="E130" t="s">
+        <v>203</v>
       </c>
       <c r="F130" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="131" spans="2:9" x14ac:dyDescent="0.3">
@@ -4274,10 +4487,16 @@
         <v>35</v>
       </c>
       <c r="C133" t="s">
-        <v>186</v>
+        <v>185</v>
+      </c>
+      <c r="D133" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="E133" t="s">
+        <v>203</v>
       </c>
       <c r="F133" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="134" spans="2:9" x14ac:dyDescent="0.3">
@@ -4295,10 +4514,16 @@
         <v>36</v>
       </c>
       <c r="C136" t="s">
-        <v>186</v>
+        <v>185</v>
+      </c>
+      <c r="D136" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="E136" t="s">
+        <v>203</v>
       </c>
       <c r="F136" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="137" spans="2:9" x14ac:dyDescent="0.3">
@@ -4313,16 +4538,16 @@
     </row>
     <row r="141" spans="2:9" x14ac:dyDescent="0.3">
       <c r="F141" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="G141" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="H141" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="I141" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
     </row>
     <row r="142" spans="2:9" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
[client & docs] fix client warning, move key path, and update docs
fix client warning, move key path, and update docs
</commit_message>
<xml_diff>
--- a/docs/09_static_analysis/static_analysis_20210614_v0.5.0_reviewed.xlsx
+++ b/docs/09_static_analysis/static_analysis_20210614_v0.5.0_reviewed.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\study\security\cmu\temp\cmu_project\docs\09_static_analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\17Z990_PC5\Downloads\security_specialist\03.cmu\project\cmu_project\docs\09_static_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12390" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12390"/>
   </bookViews>
   <sheets>
     <sheet name="cppchecker_20210614_v0.5.0" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="655" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="658" uniqueCount="218">
   <si>
     <t>File</t>
   </si>
@@ -702,6 +702,22 @@
   </si>
   <si>
     <t>don't calculate twice</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>delete file</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>done</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>done</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>done</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1319,7 +1335,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1333,6 +1349,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="6">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="8">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1659,19 +1681,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G101"/>
   <sheetViews>
-    <sheetView topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="A103" sqref="A103"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="108.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="108.08203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.75" customWidth="1"/>
     <col min="6" max="6" width="19.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1694,7 +1716,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>115</v>
       </c>
@@ -1711,7 +1733,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>116</v>
       </c>
@@ -1728,7 +1750,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>116</v>
       </c>
@@ -1745,7 +1767,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>120</v>
       </c>
@@ -1762,7 +1784,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>120</v>
       </c>
@@ -1779,7 +1801,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>123</v>
       </c>
@@ -1796,7 +1818,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>123</v>
       </c>
@@ -1813,7 +1835,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>126</v>
       </c>
@@ -1830,7 +1852,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>127</v>
       </c>
@@ -1847,7 +1869,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>127</v>
       </c>
@@ -1864,7 +1886,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>127</v>
       </c>
@@ -1881,7 +1903,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>128</v>
       </c>
@@ -1898,7 +1920,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>128</v>
       </c>
@@ -1915,7 +1937,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>128</v>
       </c>
@@ -1932,7 +1954,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>128</v>
       </c>
@@ -1949,7 +1971,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>128</v>
       </c>
@@ -1966,7 +1988,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>128</v>
       </c>
@@ -1983,7 +2005,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>128</v>
       </c>
@@ -2000,7 +2022,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>128</v>
       </c>
@@ -2017,7 +2039,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>128</v>
       </c>
@@ -2034,7 +2056,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>128</v>
       </c>
@@ -2051,7 +2073,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>128</v>
       </c>
@@ -2068,7 +2090,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>128</v>
       </c>
@@ -2085,7 +2107,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>128</v>
       </c>
@@ -2102,7 +2124,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>128</v>
       </c>
@@ -2119,7 +2141,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>128</v>
       </c>
@@ -2136,7 +2158,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>129</v>
       </c>
@@ -2153,7 +2175,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>129</v>
       </c>
@@ -2170,7 +2192,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>130</v>
       </c>
@@ -2187,7 +2209,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>130</v>
       </c>
@@ -2204,7 +2226,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>131</v>
       </c>
@@ -2221,7 +2243,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>132</v>
       </c>
@@ -2238,7 +2260,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>132</v>
       </c>
@@ -2255,7 +2277,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>132</v>
       </c>
@@ -2272,7 +2294,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>133</v>
       </c>
@@ -2289,7 +2311,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>133</v>
       </c>
@@ -2306,7 +2328,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
         <v>133</v>
       </c>
@@ -2323,7 +2345,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>137</v>
       </c>
@@ -2340,7 +2362,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
         <v>137</v>
       </c>
@@ -2357,7 +2379,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
         <v>137</v>
       </c>
@@ -2374,7 +2396,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
         <v>137</v>
       </c>
@@ -2391,7 +2413,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
         <v>137</v>
       </c>
@@ -2408,7 +2430,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
         <v>137</v>
       </c>
@@ -2425,7 +2447,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
         <v>137</v>
       </c>
@@ -2442,7 +2464,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
         <v>137</v>
       </c>
@@ -2459,7 +2481,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
         <v>137</v>
       </c>
@@ -2476,7 +2498,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
         <v>138</v>
       </c>
@@ -2493,7 +2515,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
         <v>138</v>
       </c>
@@ -2510,7 +2532,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
         <v>138</v>
       </c>
@@ -2527,7 +2549,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
         <v>138</v>
       </c>
@@ -2544,7 +2566,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
         <v>138</v>
       </c>
@@ -2561,7 +2583,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
         <v>138</v>
       </c>
@@ -2578,7 +2600,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
         <v>138</v>
       </c>
@@ -2595,7 +2617,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
         <v>138</v>
       </c>
@@ -2612,7 +2634,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
         <v>138</v>
       </c>
@@ -2629,7 +2651,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
         <v>138</v>
       </c>
@@ -2646,7 +2668,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
         <v>138</v>
       </c>
@@ -2663,7 +2685,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
         <v>138</v>
       </c>
@@ -2680,7 +2702,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
         <v>138</v>
       </c>
@@ -2697,7 +2719,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
         <v>139</v>
       </c>
@@ -2714,7 +2736,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
         <v>139</v>
       </c>
@@ -2731,7 +2753,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
         <v>139</v>
       </c>
@@ -2748,7 +2770,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
         <v>140</v>
       </c>
@@ -2765,7 +2787,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
         <v>140</v>
       </c>
@@ -2782,7 +2804,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
         <v>140</v>
       </c>
@@ -2799,7 +2821,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
         <v>141</v>
       </c>
@@ -2816,7 +2838,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
         <v>141</v>
       </c>
@@ -2833,7 +2855,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
         <v>141</v>
       </c>
@@ -2850,7 +2872,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
         <v>142</v>
       </c>
@@ -2867,7 +2889,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
         <v>142</v>
       </c>
@@ -2884,7 +2906,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
         <v>142</v>
       </c>
@@ -2901,7 +2923,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
         <v>142</v>
       </c>
@@ -2918,7 +2940,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
         <v>142</v>
       </c>
@@ -2935,7 +2957,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
         <v>142</v>
       </c>
@@ -2952,7 +2974,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A76" t="s">
         <v>142</v>
       </c>
@@ -2969,7 +2991,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A77" t="s">
         <v>142</v>
       </c>
@@ -2986,7 +3008,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A78" t="s">
         <v>143</v>
       </c>
@@ -3003,7 +3025,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A79" t="s">
         <v>143</v>
       </c>
@@ -3020,7 +3042,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A80" t="s">
         <v>143</v>
       </c>
@@ -3037,7 +3059,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A81" t="s">
         <v>143</v>
       </c>
@@ -3054,7 +3076,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A82" t="s">
         <v>143</v>
       </c>
@@ -3071,7 +3093,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A83" t="s">
         <v>143</v>
       </c>
@@ -3088,7 +3110,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A84" t="s">
         <v>143</v>
       </c>
@@ -3105,7 +3127,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A85" t="s">
         <v>143</v>
       </c>
@@ -3122,7 +3144,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A86" t="s">
         <v>143</v>
       </c>
@@ -3139,7 +3161,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A87" t="s">
         <v>143</v>
       </c>
@@ -3156,7 +3178,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A88" t="s">
         <v>143</v>
       </c>
@@ -3173,7 +3195,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A89" t="s">
         <v>143</v>
       </c>
@@ -3190,7 +3212,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A90" t="s">
         <v>143</v>
       </c>
@@ -3207,7 +3229,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A91" t="s">
         <v>143</v>
       </c>
@@ -3224,7 +3246,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A92" t="s">
         <v>143</v>
       </c>
@@ -3241,7 +3263,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A93" t="s">
         <v>143</v>
       </c>
@@ -3258,7 +3280,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A94" t="s">
         <v>143</v>
       </c>
@@ -3275,7 +3297,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A95" t="s">
         <v>143</v>
       </c>
@@ -3292,7 +3314,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A96" t="s">
         <v>143</v>
       </c>
@@ -3309,7 +3331,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A97" t="s">
         <v>143</v>
       </c>
@@ -3326,7 +3348,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A98" t="s">
         <v>143</v>
       </c>
@@ -3343,7 +3365,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A99" t="s">
         <v>143</v>
       </c>
@@ -3360,7 +3382,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A100" t="s">
         <v>143</v>
       </c>
@@ -3377,7 +3399,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A101" t="s">
         <v>144</v>
       </c>
@@ -3406,21 +3428,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:W142"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="2" width="12" customWidth="1"/>
-    <col min="3" max="3" width="10.875" customWidth="1"/>
-    <col min="5" max="5" width="12.375" customWidth="1"/>
-    <col min="6" max="6" width="12.625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.625" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" customWidth="1"/>
+    <col min="6" max="6" width="12.58203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.58203125" customWidth="1"/>
     <col min="8" max="8" width="18.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>178</v>
       </c>
@@ -3434,14 +3456,14 @@
         <v>180</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5" t="s">
         <v>182</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="6" t="s">
         <v>206</v>
       </c>
       <c r="E5" t="s">
@@ -3451,37 +3473,37 @@
         <v>181</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F6" t="s">
         <v>98</v>
       </c>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F7" t="s">
         <v>99</v>
       </c>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F8" t="s">
         <v>100</v>
       </c>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F9" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B10">
         <v>2</v>
       </c>
       <c r="C10" t="s">
         <v>182</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="6" t="s">
         <v>206</v>
       </c>
       <c r="E10" t="s">
@@ -3491,33 +3513,36 @@
         <v>145</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F11" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F12" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F13" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F14" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B15">
         <v>3</v>
       </c>
       <c r="C15" t="s">
         <v>182</v>
       </c>
+      <c r="D15" s="5" t="s">
+        <v>215</v>
+      </c>
       <c r="E15" t="s">
         <v>204</v>
       </c>
@@ -3525,33 +3550,36 @@
         <v>146</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F16" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.45">
       <c r="F17" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.45">
       <c r="F18" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.45">
       <c r="F19" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B20">
         <v>4</v>
       </c>
       <c r="C20" t="s">
         <v>182</v>
       </c>
+      <c r="D20" s="5" t="s">
+        <v>215</v>
+      </c>
       <c r="E20" t="s">
         <v>204</v>
       </c>
@@ -3559,33 +3587,36 @@
         <v>147</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.45">
       <c r="F21" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.45">
       <c r="F22" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.45">
       <c r="F23" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.45">
       <c r="F24" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B25">
         <v>5</v>
       </c>
       <c r="C25" t="s">
         <v>182</v>
       </c>
+      <c r="D25" s="5" t="s">
+        <v>215</v>
+      </c>
       <c r="E25" t="s">
         <v>204</v>
       </c>
@@ -3593,34 +3624,34 @@
         <v>148</v>
       </c>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.45">
       <c r="F26" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.45">
       <c r="F27" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.45">
       <c r="F28" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="29" spans="2:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:6" s="3" customFormat="1" x14ac:dyDescent="0.45">
       <c r="F29" s="3" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="30" spans="2:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:6" s="3" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B30" s="3">
         <v>6</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="D30" s="3" t="s">
+      <c r="D30" s="6" t="s">
         <v>206</v>
       </c>
       <c r="E30" s="3" t="s">
@@ -3630,24 +3661,24 @@
         <v>191</v>
       </c>
     </row>
-    <row r="31" spans="2:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:6" s="3" customFormat="1" x14ac:dyDescent="0.45">
       <c r="F31" s="3" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="32" spans="2:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:6" s="3" customFormat="1" x14ac:dyDescent="0.45">
       <c r="F32" s="3" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="33" spans="2:23" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:23" s="3" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B33" s="3">
         <v>7</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="D33" s="3" t="s">
+      <c r="D33" s="6" t="s">
         <v>206</v>
       </c>
       <c r="E33" s="3" t="s">
@@ -3657,130 +3688,130 @@
         <v>149</v>
       </c>
     </row>
-    <row r="34" spans="2:23" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:23" s="3" customFormat="1" x14ac:dyDescent="0.45">
       <c r="F34" s="3" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="35" spans="2:23" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:23" s="3" customFormat="1" x14ac:dyDescent="0.45">
       <c r="F35" s="3" t="s">
         <v>103</v>
       </c>
       <c r="W35" s="4"/>
     </row>
-    <row r="36" spans="2:23" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:23" s="3" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B36" s="3">
         <v>8</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="D36" s="3" t="s">
+      <c r="D36" s="6" t="s">
         <v>206</v>
       </c>
       <c r="E36" t="s">
-        <v>203</v>
+        <v>214</v>
       </c>
       <c r="F36" s="3" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="37" spans="2:23" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:23" s="3" customFormat="1" x14ac:dyDescent="0.45">
       <c r="F37" s="3" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="38" spans="2:23" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:23" s="3" customFormat="1" x14ac:dyDescent="0.45">
       <c r="F38" s="3" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="39" spans="2:23" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:23" s="3" customFormat="1" x14ac:dyDescent="0.45">
       <c r="F39" s="3" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="40" spans="2:23" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:23" s="3" customFormat="1" x14ac:dyDescent="0.45">
       <c r="F40" s="3" t="s">
         <v>101</v>
       </c>
       <c r="W40" s="4"/>
     </row>
-    <row r="41" spans="2:23" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:23" s="3" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B41" s="3">
         <v>9</v>
       </c>
       <c r="C41" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="D41" s="3" t="s">
+      <c r="D41" s="6" t="s">
         <v>206</v>
       </c>
       <c r="E41" t="s">
-        <v>203</v>
+        <v>214</v>
       </c>
       <c r="F41" s="3" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="42" spans="2:23" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:23" s="3" customFormat="1" x14ac:dyDescent="0.45">
       <c r="F42" s="3" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="43" spans="2:23" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:23" s="3" customFormat="1" x14ac:dyDescent="0.45">
       <c r="F43" s="3" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="44" spans="2:23" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:23" s="3" customFormat="1" x14ac:dyDescent="0.45">
       <c r="F44" s="3" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="45" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:23" x14ac:dyDescent="0.45">
       <c r="F45" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="46" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:23" x14ac:dyDescent="0.45">
       <c r="B46">
         <v>10</v>
       </c>
       <c r="C46" t="s">
         <v>182</v>
       </c>
-      <c r="D46" s="3" t="s">
+      <c r="D46" s="6" t="s">
         <v>206</v>
       </c>
       <c r="E46" t="s">
-        <v>203</v>
+        <v>214</v>
       </c>
       <c r="F46" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="47" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:23" x14ac:dyDescent="0.45">
       <c r="F47" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="48" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:23" x14ac:dyDescent="0.45">
       <c r="F48" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="49" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:14" x14ac:dyDescent="0.45">
       <c r="F49" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="50" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:14" x14ac:dyDescent="0.45">
       <c r="F50" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="51" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B51">
         <v>11</v>
       </c>
@@ -3797,27 +3828,27 @@
         <v>152</v>
       </c>
     </row>
-    <row r="52" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:14" x14ac:dyDescent="0.45">
       <c r="F52" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="53" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:14" x14ac:dyDescent="0.45">
       <c r="F53" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="54" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:14" x14ac:dyDescent="0.45">
       <c r="F54" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="55" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:14" x14ac:dyDescent="0.45">
       <c r="F55" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="56" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B56">
         <v>12</v>
       </c>
@@ -3834,27 +3865,27 @@
         <v>153</v>
       </c>
     </row>
-    <row r="57" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:14" x14ac:dyDescent="0.45">
       <c r="F57" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="58" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:14" x14ac:dyDescent="0.45">
       <c r="F58" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="59" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:14" x14ac:dyDescent="0.45">
       <c r="F59" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="60" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:14" x14ac:dyDescent="0.45">
       <c r="F60" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="61" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B61">
         <v>13</v>
       </c>
@@ -3874,34 +3905,34 @@
         <v>212</v>
       </c>
     </row>
-    <row r="62" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:14" x14ac:dyDescent="0.45">
       <c r="F62" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="63" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:14" x14ac:dyDescent="0.45">
       <c r="F63" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="64" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:14" x14ac:dyDescent="0.45">
       <c r="F64" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="65" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:6" x14ac:dyDescent="0.45">
       <c r="F65" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="66" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B66">
         <v>14</v>
       </c>
       <c r="C66" t="s">
         <v>187</v>
       </c>
-      <c r="D66" s="3" t="s">
+      <c r="D66" s="6" t="s">
         <v>206</v>
       </c>
       <c r="E66" s="3" t="s">
@@ -3911,24 +3942,24 @@
         <v>155</v>
       </c>
     </row>
-    <row r="67" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:6" x14ac:dyDescent="0.45">
       <c r="F67" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="68" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:6" x14ac:dyDescent="0.45">
       <c r="F68" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="69" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B69">
         <v>15</v>
       </c>
       <c r="C69" t="s">
         <v>188</v>
       </c>
-      <c r="D69" s="3" t="s">
+      <c r="D69" s="6" t="s">
         <v>206</v>
       </c>
       <c r="E69" s="3" t="s">
@@ -3938,17 +3969,17 @@
         <v>156</v>
       </c>
     </row>
-    <row r="70" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:6" x14ac:dyDescent="0.45">
       <c r="F70" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="71" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:6" x14ac:dyDescent="0.45">
       <c r="F71" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="72" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B72">
         <v>16</v>
       </c>
@@ -3965,27 +3996,27 @@
         <v>157</v>
       </c>
     </row>
-    <row r="73" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:6" x14ac:dyDescent="0.45">
       <c r="F73" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="74" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:6" x14ac:dyDescent="0.45">
       <c r="F74" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="75" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:6" x14ac:dyDescent="0.45">
       <c r="F75" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="76" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="76" spans="2:6" x14ac:dyDescent="0.45">
       <c r="F76" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="77" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="77" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B77">
         <v>17</v>
       </c>
@@ -4002,34 +4033,34 @@
         <v>193</v>
       </c>
     </row>
-    <row r="78" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:6" x14ac:dyDescent="0.45">
       <c r="F78" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="79" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="79" spans="2:6" x14ac:dyDescent="0.45">
       <c r="F79" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="80" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:6" x14ac:dyDescent="0.45">
       <c r="F80" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="81" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="81" spans="2:23" x14ac:dyDescent="0.45">
       <c r="F81" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="82" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="82" spans="2:23" x14ac:dyDescent="0.45">
       <c r="B82">
         <v>18</v>
       </c>
       <c r="C82" t="s">
         <v>182</v>
       </c>
-      <c r="D82" s="3" t="s">
+      <c r="D82" s="6" t="s">
         <v>206</v>
       </c>
       <c r="E82" t="s">
@@ -4039,24 +4070,24 @@
         <v>194</v>
       </c>
     </row>
-    <row r="83" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="83" spans="2:23" x14ac:dyDescent="0.45">
       <c r="F83" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="84" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="84" spans="2:23" x14ac:dyDescent="0.45">
       <c r="F84" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="85" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="85" spans="2:23" x14ac:dyDescent="0.45">
       <c r="B85">
         <v>19</v>
       </c>
       <c r="C85" t="s">
         <v>182</v>
       </c>
-      <c r="D85" s="3" t="s">
+      <c r="D85" s="6" t="s">
         <v>206</v>
       </c>
       <c r="E85" t="s">
@@ -4066,25 +4097,25 @@
         <v>160</v>
       </c>
     </row>
-    <row r="86" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="86" spans="2:23" x14ac:dyDescent="0.45">
       <c r="F86" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="87" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="87" spans="2:23" x14ac:dyDescent="0.45">
       <c r="F87" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="88" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="88" spans="2:23" x14ac:dyDescent="0.45">
       <c r="B88">
         <v>20</v>
       </c>
       <c r="C88" t="s">
         <v>182</v>
       </c>
-      <c r="D88" t="s">
-        <v>209</v>
+      <c r="D88" s="5" t="s">
+        <v>216</v>
       </c>
       <c r="E88" t="s">
         <v>213</v>
@@ -4093,25 +4124,25 @@
         <v>161</v>
       </c>
     </row>
-    <row r="89" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="89" spans="2:23" x14ac:dyDescent="0.45">
       <c r="F89" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="90" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="90" spans="2:23" x14ac:dyDescent="0.45">
       <c r="F90" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="91" spans="2:23" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="2:23" s="3" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B91" s="3">
         <v>21</v>
       </c>
       <c r="C91" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="D91" t="s">
-        <v>209</v>
+      <c r="D91" s="5" t="s">
+        <v>217</v>
       </c>
       <c r="E91" t="s">
         <v>213</v>
@@ -4121,17 +4152,17 @@
       </c>
       <c r="W91" s="4"/>
     </row>
-    <row r="92" spans="2:23" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="2:23" s="3" customFormat="1" x14ac:dyDescent="0.45">
       <c r="F92" s="3" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="93" spans="2:23" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="2:23" s="3" customFormat="1" x14ac:dyDescent="0.45">
       <c r="F93" s="3" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="94" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="94" spans="2:23" x14ac:dyDescent="0.45">
       <c r="B94">
         <v>22</v>
       </c>
@@ -4148,17 +4179,17 @@
         <v>163</v>
       </c>
     </row>
-    <row r="95" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="95" spans="2:23" x14ac:dyDescent="0.45">
       <c r="F95" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="96" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="96" spans="2:23" x14ac:dyDescent="0.45">
       <c r="F96" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="97" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="97" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B97">
         <v>23</v>
       </c>
@@ -4175,98 +4206,98 @@
         <v>164</v>
       </c>
     </row>
-    <row r="98" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="98" spans="2:6" x14ac:dyDescent="0.45">
       <c r="F98" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="99" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="99" spans="2:6" x14ac:dyDescent="0.45">
       <c r="F99" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="100" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="100" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B100">
         <v>24</v>
       </c>
       <c r="C100" t="s">
         <v>182</v>
       </c>
-      <c r="D100" s="3" t="s">
+      <c r="D100" s="6" t="s">
         <v>206</v>
       </c>
       <c r="E100" t="s">
-        <v>203</v>
+        <v>214</v>
       </c>
       <c r="F100" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="101" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="101" spans="2:6" x14ac:dyDescent="0.45">
       <c r="F101" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="102" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="102" spans="2:6" x14ac:dyDescent="0.45">
       <c r="F102" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="103" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="103" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B103">
         <v>25</v>
       </c>
       <c r="C103" t="s">
         <v>182</v>
       </c>
-      <c r="D103" s="3" t="s">
+      <c r="D103" s="6" t="s">
         <v>206</v>
       </c>
       <c r="E103" t="s">
-        <v>203</v>
+        <v>214</v>
       </c>
       <c r="F103" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="104" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="104" spans="2:6" x14ac:dyDescent="0.45">
       <c r="F104" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="105" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="105" spans="2:6" x14ac:dyDescent="0.45">
       <c r="F105" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="106" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="106" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B106">
         <v>26</v>
       </c>
       <c r="C106" t="s">
         <v>196</v>
       </c>
-      <c r="D106" s="3" t="s">
+      <c r="D106" s="6" t="s">
         <v>206</v>
       </c>
       <c r="E106" t="s">
-        <v>203</v>
+        <v>214</v>
       </c>
       <c r="F106" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="107" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="107" spans="2:6" x14ac:dyDescent="0.45">
       <c r="F107" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="108" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="108" spans="2:6" x14ac:dyDescent="0.45">
       <c r="F108" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="109" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="109" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B109">
         <v>27</v>
       </c>
@@ -4283,17 +4314,17 @@
         <v>168</v>
       </c>
     </row>
-    <row r="110" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="110" spans="2:6" x14ac:dyDescent="0.45">
       <c r="F110" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="111" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="111" spans="2:6" x14ac:dyDescent="0.45">
       <c r="F111" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="112" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="112" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B112">
         <v>28</v>
       </c>
@@ -4310,17 +4341,17 @@
         <v>169</v>
       </c>
     </row>
-    <row r="113" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="113" spans="2:6" x14ac:dyDescent="0.45">
       <c r="F113" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="114" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="114" spans="2:6" x14ac:dyDescent="0.45">
       <c r="F114" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="115" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="115" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B115">
         <v>29</v>
       </c>
@@ -4337,17 +4368,17 @@
         <v>170</v>
       </c>
     </row>
-    <row r="116" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="116" spans="2:6" x14ac:dyDescent="0.45">
       <c r="F116" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="117" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="117" spans="2:6" x14ac:dyDescent="0.45">
       <c r="F117" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="118" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="118" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B118">
         <v>30</v>
       </c>
@@ -4364,17 +4395,17 @@
         <v>171</v>
       </c>
     </row>
-    <row r="119" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="119" spans="2:6" x14ac:dyDescent="0.45">
       <c r="F119" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="120" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="120" spans="2:6" x14ac:dyDescent="0.45">
       <c r="F120" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="121" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="121" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B121">
         <v>31</v>
       </c>
@@ -4391,17 +4422,17 @@
         <v>172</v>
       </c>
     </row>
-    <row r="122" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="122" spans="2:6" x14ac:dyDescent="0.45">
       <c r="F122" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="123" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="123" spans="2:6" x14ac:dyDescent="0.45">
       <c r="F123" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="124" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="124" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B124">
         <v>32</v>
       </c>
@@ -4418,17 +4449,17 @@
         <v>173</v>
       </c>
     </row>
-    <row r="125" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="125" spans="2:6" x14ac:dyDescent="0.45">
       <c r="F125" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="126" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="126" spans="2:6" x14ac:dyDescent="0.45">
       <c r="F126" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="127" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="127" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B127">
         <v>33</v>
       </c>
@@ -4445,17 +4476,17 @@
         <v>174</v>
       </c>
     </row>
-    <row r="128" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="128" spans="2:6" x14ac:dyDescent="0.45">
       <c r="F128" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="129" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="129" spans="2:9" x14ac:dyDescent="0.45">
       <c r="F129" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="130" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="130" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B130">
         <v>34</v>
       </c>
@@ -4472,17 +4503,17 @@
         <v>175</v>
       </c>
     </row>
-    <row r="131" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="131" spans="2:9" x14ac:dyDescent="0.45">
       <c r="F131" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="132" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="132" spans="2:9" x14ac:dyDescent="0.45">
       <c r="F132" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="133" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="133" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B133">
         <v>35</v>
       </c>
@@ -4499,17 +4530,17 @@
         <v>176</v>
       </c>
     </row>
-    <row r="134" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="134" spans="2:9" x14ac:dyDescent="0.45">
       <c r="F134" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="135" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="135" spans="2:9" x14ac:dyDescent="0.45">
       <c r="F135" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="136" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="136" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B136">
         <v>36</v>
       </c>
@@ -4526,17 +4557,17 @@
         <v>177</v>
       </c>
     </row>
-    <row r="137" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="137" spans="2:9" x14ac:dyDescent="0.45">
       <c r="F137" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="138" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="138" spans="2:9" x14ac:dyDescent="0.45">
       <c r="F138" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="141" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="141" spans="2:9" x14ac:dyDescent="0.45">
       <c r="F141" t="s">
         <v>199</v>
       </c>
@@ -4550,7 +4581,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="142" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="142" spans="2:9" x14ac:dyDescent="0.45">
       <c r="F142">
         <v>36</v>
       </c>

</xml_diff>

<commit_message>
[docs] update static analysis v0.5.0
update static analysis v0.5.0
</commit_message>
<xml_diff>
--- a/docs/09_static_analysis/static_analysis_20210614_v0.5.0_reviewed.xlsx
+++ b/docs/09_static_analysis/static_analysis_20210614_v0.5.0_reviewed.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\17Z990_PC5\Downloads\security_specialist\03.cmu\project\cmu_project\docs\09_static_analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\study\security\cmu\temp\cmu_project\docs\09_static_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="658" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="221">
   <si>
     <t>File</t>
   </si>
@@ -718,6 +718,18 @@
   </si>
   <si>
     <t>done</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">closed </t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Id</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>number</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1416,6 +1428,1214 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="ko-KR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'cppchecker_20210614_v0.5.0'!$F$108</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>number</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="317500" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="25000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="317500" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="25000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="317500" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="25000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="317500" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="25000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="317500" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="25000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="317500" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="25000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="317500" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="25000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="7"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="317500" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="25000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="8"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="317500" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="25000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="9"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="317500" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="25000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="10"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="317500" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="25000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="11"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="317500" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="25000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="12"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="317500" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="25000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="13"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="317500" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="25000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="14"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="317500" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="25000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="ko-KR"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="inEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="35000"/>
+                      <a:lumOff val="65000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:round/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:leaderLines>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'cppchecker_20210614_v0.5.0'!$E$109:$E$123</c:f>
+              <c:strCache>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>constParameter</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>invalidPointerCast</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>knownConditionTrueFalse</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>missingOverride</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>noCopyConstructor</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>noExplicitConstructor</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>noOperatorEq</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>passedByValue</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>postfixOperator</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>uninitMemberVar</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>unreadVariable</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>unusedFunction</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>unusedLabel</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>useInitializationList</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>variableScope</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'cppchecker_20210614_v0.5.0'!$F$109:$F$123</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="inEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="1"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="78000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ko-KR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:pattFill prst="dkDnDiag">
+      <a:fgClr>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="95000"/>
+        </a:schemeClr>
+      </a:fgClr>
+      <a:bgClr>
+        <a:schemeClr val="lt1"/>
+      </a:bgClr>
+    </a:pattFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ko-KR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="261">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="dkDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:alpha val="75000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="317500" algn="ctr" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="25000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="88900" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="20000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+      <a:scene3d>
+        <a:camera prst="orthographicFront"/>
+        <a:lightRig rig="threePt" dir="t"/>
+      </a:scene3d>
+      <a:sp3d prstMaterial="matte"/>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:alpha val="78000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1800" b="1" kern="1200" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1600200</xdr:colOff>
+      <xdr:row>104</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>126</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="차트 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 테마">
   <a:themeElements>
@@ -1679,21 +2899,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G101"/>
+  <dimension ref="A1:H123"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="D126" sqref="D126"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="108.08203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="108.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.75" customWidth="1"/>
     <col min="6" max="6" width="19.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1716,7 +2936,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>115</v>
       </c>
@@ -1733,7 +2953,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>116</v>
       </c>
@@ -1750,7 +2970,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>116</v>
       </c>
@@ -1767,7 +2987,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>120</v>
       </c>
@@ -1784,7 +3004,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>120</v>
       </c>
@@ -1801,7 +3021,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>123</v>
       </c>
@@ -1818,7 +3038,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>123</v>
       </c>
@@ -1835,7 +3055,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>126</v>
       </c>
@@ -1852,7 +3072,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>127</v>
       </c>
@@ -1869,7 +3089,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>127</v>
       </c>
@@ -1886,7 +3106,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>127</v>
       </c>
@@ -1903,7 +3123,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>128</v>
       </c>
@@ -1920,7 +3140,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>128</v>
       </c>
@@ -1937,7 +3157,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>128</v>
       </c>
@@ -1954,7 +3174,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>128</v>
       </c>
@@ -1971,7 +3191,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>128</v>
       </c>
@@ -1988,7 +3208,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>128</v>
       </c>
@@ -2005,7 +3225,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>128</v>
       </c>
@@ -2022,7 +3242,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>128</v>
       </c>
@@ -2039,7 +3259,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>128</v>
       </c>
@@ -2056,7 +3276,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>128</v>
       </c>
@@ -2073,7 +3293,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>128</v>
       </c>
@@ -2090,7 +3310,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>128</v>
       </c>
@@ -2107,7 +3327,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>128</v>
       </c>
@@ -2124,7 +3344,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>128</v>
       </c>
@@ -2141,7 +3361,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>128</v>
       </c>
@@ -2158,7 +3378,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>129</v>
       </c>
@@ -2175,7 +3395,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>129</v>
       </c>
@@ -2192,7 +3412,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>130</v>
       </c>
@@ -2209,7 +3429,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>130</v>
       </c>
@@ -2226,7 +3446,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>131</v>
       </c>
@@ -2243,7 +3463,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>132</v>
       </c>
@@ -2260,7 +3480,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>132</v>
       </c>
@@ -2277,7 +3497,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>132</v>
       </c>
@@ -2294,7 +3514,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>133</v>
       </c>
@@ -2311,7 +3531,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>133</v>
       </c>
@@ -2328,7 +3548,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>133</v>
       </c>
@@ -2345,7 +3565,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>137</v>
       </c>
@@ -2362,7 +3582,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>137</v>
       </c>
@@ -2379,7 +3599,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>137</v>
       </c>
@@ -2396,7 +3616,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>137</v>
       </c>
@@ -2413,7 +3633,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>137</v>
       </c>
@@ -2430,7 +3650,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>137</v>
       </c>
@@ -2447,7 +3667,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>137</v>
       </c>
@@ -2464,7 +3684,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>137</v>
       </c>
@@ -2481,7 +3701,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>137</v>
       </c>
@@ -2498,7 +3718,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>138</v>
       </c>
@@ -2515,7 +3735,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>138</v>
       </c>
@@ -2532,7 +3752,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>138</v>
       </c>
@@ -2549,7 +3769,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>138</v>
       </c>
@@ -2566,7 +3786,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>138</v>
       </c>
@@ -2583,7 +3803,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>138</v>
       </c>
@@ -2600,7 +3820,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>138</v>
       </c>
@@ -2617,7 +3837,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>138</v>
       </c>
@@ -2634,7 +3854,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>138</v>
       </c>
@@ -2651,7 +3871,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>138</v>
       </c>
@@ -2668,7 +3888,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>138</v>
       </c>
@@ -2685,7 +3905,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>138</v>
       </c>
@@ -2702,7 +3922,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>138</v>
       </c>
@@ -2719,7 +3939,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>139</v>
       </c>
@@ -2736,7 +3956,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>139</v>
       </c>
@@ -2753,7 +3973,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>139</v>
       </c>
@@ -2770,7 +3990,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>140</v>
       </c>
@@ -2787,7 +4007,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>140</v>
       </c>
@@ -2804,7 +4024,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>140</v>
       </c>
@@ -2821,7 +4041,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>141</v>
       </c>
@@ -2838,7 +4058,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>141</v>
       </c>
@@ -2855,7 +4075,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>141</v>
       </c>
@@ -2872,7 +4092,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>142</v>
       </c>
@@ -2889,7 +4109,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>142</v>
       </c>
@@ -2906,7 +4126,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>142</v>
       </c>
@@ -2923,7 +4143,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>142</v>
       </c>
@@ -2940,7 +4160,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>142</v>
       </c>
@@ -2957,7 +4177,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>142</v>
       </c>
@@ -2974,7 +4194,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>142</v>
       </c>
@@ -2991,7 +4211,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>142</v>
       </c>
@@ -3008,7 +4228,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>143</v>
       </c>
@@ -3025,7 +4245,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>143</v>
       </c>
@@ -3042,7 +4262,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>143</v>
       </c>
@@ -3059,7 +4279,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>143</v>
       </c>
@@ -3076,7 +4296,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>143</v>
       </c>
@@ -3093,7 +4313,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>143</v>
       </c>
@@ -3110,7 +4330,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>143</v>
       </c>
@@ -3127,7 +4347,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>143</v>
       </c>
@@ -3144,7 +4364,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>143</v>
       </c>
@@ -3161,7 +4381,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>143</v>
       </c>
@@ -3178,7 +4398,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>143</v>
       </c>
@@ -3195,7 +4415,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>143</v>
       </c>
@@ -3212,7 +4432,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>143</v>
       </c>
@@ -3229,7 +4449,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>143</v>
       </c>
@@ -3246,7 +4466,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>143</v>
       </c>
@@ -3263,7 +4483,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>143</v>
       </c>
@@ -3280,7 +4500,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>143</v>
       </c>
@@ -3297,7 +4517,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>143</v>
       </c>
@@ -3314,7 +4534,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>143</v>
       </c>
@@ -3331,7 +4551,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>143</v>
       </c>
@@ -3348,7 +4568,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>143</v>
       </c>
@@ -3365,7 +4585,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>143</v>
       </c>
@@ -3382,7 +4602,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>143</v>
       </c>
@@ -3399,7 +4619,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>144</v>
       </c>
@@ -3414,6 +4634,177 @@
       </c>
       <c r="G101" t="s">
         <v>96</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E104" t="s">
+        <v>199</v>
+      </c>
+      <c r="F104" t="s">
+        <v>200</v>
+      </c>
+      <c r="G104" t="s">
+        <v>218</v>
+      </c>
+      <c r="H104" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E105">
+        <v>100</v>
+      </c>
+      <c r="F105">
+        <v>100</v>
+      </c>
+      <c r="G105">
+        <v>0</v>
+      </c>
+      <c r="H105">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E108" t="s">
+        <v>219</v>
+      </c>
+      <c r="F108" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E109" t="s">
+        <v>41</v>
+      </c>
+      <c r="F109">
+        <f>COUNTIF(F2:F101,E109)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E110" t="s">
+        <v>95</v>
+      </c>
+      <c r="F110">
+        <f t="shared" ref="F110:F123" si="0">COUNTIF(F3:F102,E110)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E111" t="s">
+        <v>124</v>
+      </c>
+      <c r="F111">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E112" t="s">
+        <v>15</v>
+      </c>
+      <c r="F112">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="113" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E113" t="s">
+        <v>18</v>
+      </c>
+      <c r="F113">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="114" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E114" t="s">
+        <v>13</v>
+      </c>
+      <c r="F114">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="115" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E115" t="s">
+        <v>20</v>
+      </c>
+      <c r="F115">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="116" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E116" t="s">
+        <v>59</v>
+      </c>
+      <c r="F116">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="117" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E117" t="s">
+        <v>26</v>
+      </c>
+      <c r="F117">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="118" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E118" t="s">
+        <v>11</v>
+      </c>
+      <c r="F118">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="119" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E119" t="s">
+        <v>8</v>
+      </c>
+      <c r="F119">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="120" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E120" t="s">
+        <v>9</v>
+      </c>
+      <c r="F120">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="121" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E121" t="s">
+        <v>57</v>
+      </c>
+      <c r="F121">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E122" t="s">
+        <v>51</v>
+      </c>
+      <c r="F122">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="123" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E123" t="s">
+        <v>7</v>
+      </c>
+      <c r="F123">
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -3421,6 +4812,7 @@
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -3432,17 +4824,17 @@
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="12" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" customWidth="1"/>
-    <col min="5" max="5" width="12.33203125" customWidth="1"/>
-    <col min="6" max="6" width="12.58203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.58203125" customWidth="1"/>
+    <col min="3" max="3" width="10.875" customWidth="1"/>
+    <col min="5" max="5" width="12.375" customWidth="1"/>
+    <col min="6" max="6" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.625" customWidth="1"/>
     <col min="8" max="8" width="18.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>178</v>
       </c>
@@ -3456,7 +4848,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>1</v>
       </c>
@@ -3473,30 +4865,30 @@
         <v>181</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="F6" t="s">
         <v>98</v>
       </c>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="F7" t="s">
         <v>99</v>
       </c>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="F8" t="s">
         <v>100</v>
       </c>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="F9" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B10">
         <v>2</v>
       </c>
@@ -3513,27 +4905,27 @@
         <v>145</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="F11" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="F12" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="F13" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="F14" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B15">
         <v>3</v>
       </c>
@@ -3550,27 +4942,27 @@
         <v>146</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="F16" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="F17" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
       <c r="F18" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
       <c r="F19" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B20">
         <v>4</v>
       </c>
@@ -3587,27 +4979,27 @@
         <v>147</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
       <c r="F21" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
       <c r="F22" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
       <c r="F23" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
       <c r="F24" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B25">
         <v>5</v>
       </c>
@@ -3624,27 +5016,27 @@
         <v>148</v>
       </c>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
       <c r="F26" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
       <c r="F27" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
       <c r="F28" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="29" spans="2:6" s="3" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="29" spans="2:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F29" s="3" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="30" spans="2:6" s="3" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="30" spans="2:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B30" s="3">
         <v>6</v>
       </c>
@@ -3661,17 +5053,17 @@
         <v>191</v>
       </c>
     </row>
-    <row r="31" spans="2:6" s="3" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="31" spans="2:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F31" s="3" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="32" spans="2:6" s="3" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="32" spans="2:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F32" s="3" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="33" spans="2:23" s="3" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="33" spans="2:23" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B33" s="3">
         <v>7</v>
       </c>
@@ -3688,18 +5080,18 @@
         <v>149</v>
       </c>
     </row>
-    <row r="34" spans="2:23" s="3" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="34" spans="2:23" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F34" s="3" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="35" spans="2:23" s="3" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="35" spans="2:23" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F35" s="3" t="s">
         <v>103</v>
       </c>
       <c r="W35" s="4"/>
     </row>
-    <row r="36" spans="2:23" s="3" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="36" spans="2:23" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B36" s="3">
         <v>8</v>
       </c>
@@ -3716,28 +5108,28 @@
         <v>150</v>
       </c>
     </row>
-    <row r="37" spans="2:23" s="3" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="37" spans="2:23" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F37" s="3" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="38" spans="2:23" s="3" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="38" spans="2:23" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F38" s="3" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="39" spans="2:23" s="3" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="39" spans="2:23" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F39" s="3" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="40" spans="2:23" s="3" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="40" spans="2:23" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F40" s="3" t="s">
         <v>101</v>
       </c>
       <c r="W40" s="4"/>
     </row>
-    <row r="41" spans="2:23" s="3" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="41" spans="2:23" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B41" s="3">
         <v>9</v>
       </c>
@@ -3754,27 +5146,27 @@
         <v>151</v>
       </c>
     </row>
-    <row r="42" spans="2:23" s="3" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="42" spans="2:23" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F42" s="3" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="43" spans="2:23" s="3" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="43" spans="2:23" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F43" s="3" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="44" spans="2:23" s="3" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="44" spans="2:23" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F44" s="3" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="45" spans="2:23" x14ac:dyDescent="0.45">
+    <row r="45" spans="2:23" x14ac:dyDescent="0.3">
       <c r="F45" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="46" spans="2:23" x14ac:dyDescent="0.45">
+    <row r="46" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B46">
         <v>10</v>
       </c>
@@ -3791,27 +5183,27 @@
         <v>211</v>
       </c>
     </row>
-    <row r="47" spans="2:23" x14ac:dyDescent="0.45">
+    <row r="47" spans="2:23" x14ac:dyDescent="0.3">
       <c r="F47" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="48" spans="2:23" x14ac:dyDescent="0.45">
+    <row r="48" spans="2:23" x14ac:dyDescent="0.3">
       <c r="F48" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="49" spans="2:14" x14ac:dyDescent="0.45">
+    <row r="49" spans="2:14" x14ac:dyDescent="0.3">
       <c r="F49" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="50" spans="2:14" x14ac:dyDescent="0.45">
+    <row r="50" spans="2:14" x14ac:dyDescent="0.3">
       <c r="F50" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="51" spans="2:14" x14ac:dyDescent="0.45">
+    <row r="51" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B51">
         <v>11</v>
       </c>
@@ -3828,27 +5220,27 @@
         <v>152</v>
       </c>
     </row>
-    <row r="52" spans="2:14" x14ac:dyDescent="0.45">
+    <row r="52" spans="2:14" x14ac:dyDescent="0.3">
       <c r="F52" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="53" spans="2:14" x14ac:dyDescent="0.45">
+    <row r="53" spans="2:14" x14ac:dyDescent="0.3">
       <c r="F53" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="54" spans="2:14" x14ac:dyDescent="0.45">
+    <row r="54" spans="2:14" x14ac:dyDescent="0.3">
       <c r="F54" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="55" spans="2:14" x14ac:dyDescent="0.45">
+    <row r="55" spans="2:14" x14ac:dyDescent="0.3">
       <c r="F55" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="56" spans="2:14" x14ac:dyDescent="0.45">
+    <row r="56" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B56">
         <v>12</v>
       </c>
@@ -3865,27 +5257,27 @@
         <v>153</v>
       </c>
     </row>
-    <row r="57" spans="2:14" x14ac:dyDescent="0.45">
+    <row r="57" spans="2:14" x14ac:dyDescent="0.3">
       <c r="F57" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="58" spans="2:14" x14ac:dyDescent="0.45">
+    <row r="58" spans="2:14" x14ac:dyDescent="0.3">
       <c r="F58" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="59" spans="2:14" x14ac:dyDescent="0.45">
+    <row r="59" spans="2:14" x14ac:dyDescent="0.3">
       <c r="F59" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="60" spans="2:14" x14ac:dyDescent="0.45">
+    <row r="60" spans="2:14" x14ac:dyDescent="0.3">
       <c r="F60" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="61" spans="2:14" x14ac:dyDescent="0.45">
+    <row r="61" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B61">
         <v>13</v>
       </c>
@@ -3905,27 +5297,27 @@
         <v>212</v>
       </c>
     </row>
-    <row r="62" spans="2:14" x14ac:dyDescent="0.45">
+    <row r="62" spans="2:14" x14ac:dyDescent="0.3">
       <c r="F62" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="63" spans="2:14" x14ac:dyDescent="0.45">
+    <row r="63" spans="2:14" x14ac:dyDescent="0.3">
       <c r="F63" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="64" spans="2:14" x14ac:dyDescent="0.45">
+    <row r="64" spans="2:14" x14ac:dyDescent="0.3">
       <c r="F64" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="65" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="65" spans="2:6" x14ac:dyDescent="0.3">
       <c r="F65" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="66" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="66" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B66">
         <v>14</v>
       </c>
@@ -3942,17 +5334,17 @@
         <v>155</v>
       </c>
     </row>
-    <row r="67" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="67" spans="2:6" x14ac:dyDescent="0.3">
       <c r="F67" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="68" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="68" spans="2:6" x14ac:dyDescent="0.3">
       <c r="F68" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="69" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="69" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B69">
         <v>15</v>
       </c>
@@ -3969,17 +5361,17 @@
         <v>156</v>
       </c>
     </row>
-    <row r="70" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="70" spans="2:6" x14ac:dyDescent="0.3">
       <c r="F70" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="71" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="71" spans="2:6" x14ac:dyDescent="0.3">
       <c r="F71" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="72" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="72" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B72">
         <v>16</v>
       </c>
@@ -3996,27 +5388,27 @@
         <v>157</v>
       </c>
     </row>
-    <row r="73" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="73" spans="2:6" x14ac:dyDescent="0.3">
       <c r="F73" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="74" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="74" spans="2:6" x14ac:dyDescent="0.3">
       <c r="F74" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="75" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="75" spans="2:6" x14ac:dyDescent="0.3">
       <c r="F75" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="76" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="76" spans="2:6" x14ac:dyDescent="0.3">
       <c r="F76" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="77" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="77" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B77">
         <v>17</v>
       </c>
@@ -4033,27 +5425,27 @@
         <v>193</v>
       </c>
     </row>
-    <row r="78" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="78" spans="2:6" x14ac:dyDescent="0.3">
       <c r="F78" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="79" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="79" spans="2:6" x14ac:dyDescent="0.3">
       <c r="F79" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="80" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="80" spans="2:6" x14ac:dyDescent="0.3">
       <c r="F80" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="81" spans="2:23" x14ac:dyDescent="0.45">
+    <row r="81" spans="2:23" x14ac:dyDescent="0.3">
       <c r="F81" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="82" spans="2:23" x14ac:dyDescent="0.45">
+    <row r="82" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B82">
         <v>18</v>
       </c>
@@ -4070,17 +5462,17 @@
         <v>194</v>
       </c>
     </row>
-    <row r="83" spans="2:23" x14ac:dyDescent="0.45">
+    <row r="83" spans="2:23" x14ac:dyDescent="0.3">
       <c r="F83" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="84" spans="2:23" x14ac:dyDescent="0.45">
+    <row r="84" spans="2:23" x14ac:dyDescent="0.3">
       <c r="F84" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="85" spans="2:23" x14ac:dyDescent="0.45">
+    <row r="85" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B85">
         <v>19</v>
       </c>
@@ -4097,17 +5489,17 @@
         <v>160</v>
       </c>
     </row>
-    <row r="86" spans="2:23" x14ac:dyDescent="0.45">
+    <row r="86" spans="2:23" x14ac:dyDescent="0.3">
       <c r="F86" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="87" spans="2:23" x14ac:dyDescent="0.45">
+    <row r="87" spans="2:23" x14ac:dyDescent="0.3">
       <c r="F87" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="88" spans="2:23" x14ac:dyDescent="0.45">
+    <row r="88" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B88">
         <v>20</v>
       </c>
@@ -4124,17 +5516,17 @@
         <v>161</v>
       </c>
     </row>
-    <row r="89" spans="2:23" x14ac:dyDescent="0.45">
+    <row r="89" spans="2:23" x14ac:dyDescent="0.3">
       <c r="F89" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="90" spans="2:23" x14ac:dyDescent="0.45">
+    <row r="90" spans="2:23" x14ac:dyDescent="0.3">
       <c r="F90" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="91" spans="2:23" s="3" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="91" spans="2:23" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B91" s="3">
         <v>21</v>
       </c>
@@ -4152,17 +5544,17 @@
       </c>
       <c r="W91" s="4"/>
     </row>
-    <row r="92" spans="2:23" s="3" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="92" spans="2:23" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F92" s="3" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="93" spans="2:23" s="3" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="93" spans="2:23" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F93" s="3" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="94" spans="2:23" x14ac:dyDescent="0.45">
+    <row r="94" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B94">
         <v>22</v>
       </c>
@@ -4179,17 +5571,17 @@
         <v>163</v>
       </c>
     </row>
-    <row r="95" spans="2:23" x14ac:dyDescent="0.45">
+    <row r="95" spans="2:23" x14ac:dyDescent="0.3">
       <c r="F95" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="96" spans="2:23" x14ac:dyDescent="0.45">
+    <row r="96" spans="2:23" x14ac:dyDescent="0.3">
       <c r="F96" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="97" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="97" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B97">
         <v>23</v>
       </c>
@@ -4206,17 +5598,17 @@
         <v>164</v>
       </c>
     </row>
-    <row r="98" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="98" spans="2:6" x14ac:dyDescent="0.3">
       <c r="F98" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="99" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="99" spans="2:6" x14ac:dyDescent="0.3">
       <c r="F99" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="100" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="100" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B100">
         <v>24</v>
       </c>
@@ -4233,17 +5625,17 @@
         <v>165</v>
       </c>
     </row>
-    <row r="101" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="101" spans="2:6" x14ac:dyDescent="0.3">
       <c r="F101" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="102" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="102" spans="2:6" x14ac:dyDescent="0.3">
       <c r="F102" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="103" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="103" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B103">
         <v>25</v>
       </c>
@@ -4260,17 +5652,17 @@
         <v>166</v>
       </c>
     </row>
-    <row r="104" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="104" spans="2:6" x14ac:dyDescent="0.3">
       <c r="F104" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="105" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="105" spans="2:6" x14ac:dyDescent="0.3">
       <c r="F105" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="106" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="106" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B106">
         <v>26</v>
       </c>
@@ -4287,17 +5679,17 @@
         <v>167</v>
       </c>
     </row>
-    <row r="107" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="107" spans="2:6" x14ac:dyDescent="0.3">
       <c r="F107" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="108" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="108" spans="2:6" x14ac:dyDescent="0.3">
       <c r="F108" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="109" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="109" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B109">
         <v>27</v>
       </c>
@@ -4314,17 +5706,17 @@
         <v>168</v>
       </c>
     </row>
-    <row r="110" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="110" spans="2:6" x14ac:dyDescent="0.3">
       <c r="F110" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="111" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="111" spans="2:6" x14ac:dyDescent="0.3">
       <c r="F111" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="112" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="112" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B112">
         <v>28</v>
       </c>
@@ -4341,17 +5733,17 @@
         <v>169</v>
       </c>
     </row>
-    <row r="113" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="113" spans="2:6" x14ac:dyDescent="0.3">
       <c r="F113" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="114" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="114" spans="2:6" x14ac:dyDescent="0.3">
       <c r="F114" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="115" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="115" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B115">
         <v>29</v>
       </c>
@@ -4368,17 +5760,17 @@
         <v>170</v>
       </c>
     </row>
-    <row r="116" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="116" spans="2:6" x14ac:dyDescent="0.3">
       <c r="F116" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="117" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="117" spans="2:6" x14ac:dyDescent="0.3">
       <c r="F117" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="118" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="118" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B118">
         <v>30</v>
       </c>
@@ -4395,17 +5787,17 @@
         <v>171</v>
       </c>
     </row>
-    <row r="119" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="119" spans="2:6" x14ac:dyDescent="0.3">
       <c r="F119" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="120" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="120" spans="2:6" x14ac:dyDescent="0.3">
       <c r="F120" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="121" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="121" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B121">
         <v>31</v>
       </c>
@@ -4422,17 +5814,17 @@
         <v>172</v>
       </c>
     </row>
-    <row r="122" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="122" spans="2:6" x14ac:dyDescent="0.3">
       <c r="F122" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="123" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="123" spans="2:6" x14ac:dyDescent="0.3">
       <c r="F123" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="124" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="124" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B124">
         <v>32</v>
       </c>
@@ -4449,17 +5841,17 @@
         <v>173</v>
       </c>
     </row>
-    <row r="125" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="125" spans="2:6" x14ac:dyDescent="0.3">
       <c r="F125" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="126" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="126" spans="2:6" x14ac:dyDescent="0.3">
       <c r="F126" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="127" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="127" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B127">
         <v>33</v>
       </c>
@@ -4476,17 +5868,17 @@
         <v>174</v>
       </c>
     </row>
-    <row r="128" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="128" spans="2:6" x14ac:dyDescent="0.3">
       <c r="F128" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="129" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="129" spans="2:9" x14ac:dyDescent="0.3">
       <c r="F129" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="130" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="130" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B130">
         <v>34</v>
       </c>
@@ -4503,17 +5895,17 @@
         <v>175</v>
       </c>
     </row>
-    <row r="131" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="131" spans="2:9" x14ac:dyDescent="0.3">
       <c r="F131" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="132" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="132" spans="2:9" x14ac:dyDescent="0.3">
       <c r="F132" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="133" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="133" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B133">
         <v>35</v>
       </c>
@@ -4530,17 +5922,17 @@
         <v>176</v>
       </c>
     </row>
-    <row r="134" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="134" spans="2:9" x14ac:dyDescent="0.3">
       <c r="F134" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="135" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="135" spans="2:9" x14ac:dyDescent="0.3">
       <c r="F135" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="136" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="136" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B136">
         <v>36</v>
       </c>
@@ -4557,17 +5949,17 @@
         <v>177</v>
       </c>
     </row>
-    <row r="137" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="137" spans="2:9" x14ac:dyDescent="0.3">
       <c r="F137" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="138" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="138" spans="2:9" x14ac:dyDescent="0.3">
       <c r="F138" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="141" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="141" spans="2:9" x14ac:dyDescent="0.3">
       <c r="F141" t="s">
         <v>199</v>
       </c>
@@ -4581,7 +5973,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="142" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="142" spans="2:9" x14ac:dyDescent="0.3">
       <c r="F142">
         <v>36</v>
       </c>

</xml_diff>